<commit_message>
enhanced functionality of app.rb
</commit_message>
<xml_diff>
--- a/test/data.xlsx
+++ b/test/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">filename</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Fnordic walking</t>
   </si>
   <si>
-    <t xml:space="preserve">2.JPG</t>
+    <t xml:space="preserve">2.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Erich</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">„“</t>
   </si>
   <si>
-    <t xml:space="preserve">3.jpg</t>
+    <t xml:space="preserve">3.JPG</t>
   </si>
   <si>
     <t xml:space="preserve">Gustav</t>
@@ -79,10 +79,13 @@
     <t xml:space="preserve">very fnordic</t>
   </si>
   <si>
-    <t xml:space="preserve">5.jpg</t>
+    <t xml:space="preserve">5.JPG</t>
   </si>
   <si>
     <t xml:space="preserve">Anna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100.jpg</t>
   </si>
 </sst>
 </file>
@@ -188,10 +191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -274,6 +277,11 @@
         <v>20</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>